<commit_message>
Modeltyp 1 und Modeltyp 2 Modelle trainiert und evaluiert
</commit_message>
<xml_diff>
--- a/Graphics/Fehlende_Daten_pro_Station.xlsx
+++ b/Graphics/Fehlende_Daten_pro_Station.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Desktop\Maturarbeit\MA_NN_Model\Graphics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2170CFD8-B335-4F63-9863-329EE629B098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B859B95B-BA43-421B-AFB4-9470A0471AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13120" xr2:uid="{3AFE35A2-F5A5-425F-AD20-3DCB6C3E91C8}"/>
   </bookViews>
@@ -7301,7 +7301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD40CA67-42EE-4827-B8CA-6B96882E9D0C}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I42" zoomScale="77" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I39" zoomScale="77" workbookViewId="0">
       <selection activeCell="S79" sqref="S79"/>
     </sheetView>
   </sheetViews>

</xml_diff>